<commit_message>
fixed a bug with the editing of values denoted with parentheses
</commit_message>
<xml_diff>
--- a/DummySheet.xlsx
+++ b/DummySheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef774002ffc06f70/Desktop/GaugeNamProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{612FA54B-F884-4959-A2F7-CCC1BBF0844C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{074EEF74-7D66-4ED2-B2DC-17ACE0822D5F}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{612FA54B-F884-4959-A2F7-CCC1BBF0844C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADB5BC80-E444-46B5-A09C-72328220E334}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2336,22 +2336,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J582"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
+      <selection activeCell="B409" sqref="B409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>